<commit_message>
stable version with audit alerts scorecard
</commit_message>
<xml_diff>
--- a/audit_2026_1.xlsx
+++ b/audit_2026_1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,35 +434,40 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Supplier</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Invoice Qty</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Received Qty</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Rate</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Loss MT</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Loss ₹</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Leakage %</t>
         </is>
@@ -471,71 +476,121 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>testy</t>
+          <t>AS 01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>iocl</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>10</v>
+          <t>VG10</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>IOCL</t>
+        </is>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="F2" t="n">
+        <v>45</v>
+      </c>
+      <c r="G2" t="n">
         <v>50000</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
       <c r="H2" t="n">
-        <v>50000</v>
+        <v>5</v>
       </c>
       <c r="I2" t="n">
+        <v>250000</v>
+      </c>
+      <c r="J2" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>as01</t>
+          <t xml:space="preserve">TEST </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>iocl</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+          <t>VG30</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>IOCL</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3" t="n">
+        <v>50000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>VG10</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>IOML</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>50</v>
       </c>
-      <c r="E3" t="n">
-        <v>40</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="F4" t="n">
+        <v>45</v>
+      </c>
+      <c r="G4" t="n">
         <v>50000</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>250000</v>
+      </c>
+      <c r="J4" t="n">
         <v>10</v>
-      </c>
-      <c r="H3" t="n">
-        <v>500000</v>
-      </c>
-      <c r="I3" t="n">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>